<commit_message>
-code updated to implement euclidean distance -new experimental results added
</commit_message>
<xml_diff>
--- a/results/Risultati tesi v2.xlsx
+++ b/results/Risultati tesi v2.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD0DE0-5C53-4BA5-8495-4D6E648D3889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D60F1D-DBF8-48DD-BB2C-311D09B43206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MALDROID" sheetId="1" r:id="rId1"/>
-    <sheet name="MALMEM" sheetId="2" r:id="rId2"/>
+    <sheet name="MALDROID Cosine Similarity" sheetId="1" r:id="rId1"/>
+    <sheet name="MALDROID Euclidean Distance" sheetId="3" r:id="rId2"/>
+    <sheet name="MALMEM Cosine Similarity" sheetId="2" r:id="rId3"/>
+    <sheet name="MALMEM Euclidean Distance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="84">
   <si>
     <t>train_accuracy</t>
   </si>
@@ -232,6 +234,60 @@
   </si>
   <si>
     <t>110,71 hours</t>
+  </si>
+  <si>
+    <t>1,44 mins</t>
+  </si>
+  <si>
+    <t>0,58 mins</t>
+  </si>
+  <si>
+    <t>2,20 mins</t>
+  </si>
+  <si>
+    <t>10,92 mins</t>
+  </si>
+  <si>
+    <t>5,43 hours</t>
+  </si>
+  <si>
+    <t>5,60 hours</t>
+  </si>
+  <si>
+    <t>10,9 hours</t>
+  </si>
+  <si>
+    <t>14,01 hours</t>
+  </si>
+  <si>
+    <t>5,49 mins</t>
+  </si>
+  <si>
+    <t>4,59 mins</t>
+  </si>
+  <si>
+    <t>19,87 mins</t>
+  </si>
+  <si>
+    <t>4,02 mins</t>
+  </si>
+  <si>
+    <t>5,82 hours</t>
+  </si>
+  <si>
+    <t>5,58 hours</t>
+  </si>
+  <si>
+    <t>10,81 hours</t>
+  </si>
+  <si>
+    <t>14,36 hours</t>
+  </si>
+  <si>
+    <t>32,50 ,mins</t>
+  </si>
+  <si>
+    <t>29,28 days</t>
   </si>
 </sst>
 </file>
@@ -661,7 +717,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
@@ -1795,12 +1851,1150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BB75BF-02D8-44E2-A18E-419222066F54}">
+  <dimension ref="A1:U54"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="21" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2">
+        <v>0.80669999999999997</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.1003000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="F2">
+        <v>1.1375</v>
+      </c>
+      <c r="G2">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="H2">
+        <v>128</v>
+      </c>
+      <c r="I2">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="O3">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="P3">
+        <v>0.752</v>
+      </c>
+      <c r="Q3">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R3">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="S3">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="T3">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="U3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="O4">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="Q4">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0.78</v>
+      </c>
+      <c r="S4">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="T4">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="U4">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>0.753</v>
+      </c>
+      <c r="O5">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="P5">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="Q5">
+        <v>0.879</v>
+      </c>
+      <c r="R5">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="S5">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="T5">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="U5">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9">
+        <v>0.72640000000000005</v>
+      </c>
+      <c r="D9">
+        <v>1.1782999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.70069999999999999</v>
+      </c>
+      <c r="F9">
+        <v>1.2</v>
+      </c>
+      <c r="G9">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="H9">
+        <v>256</v>
+      </c>
+      <c r="I9">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="J9">
+        <v>0.7127</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10">
+        <v>0.751</v>
+      </c>
+      <c r="O10">
+        <v>0.251</v>
+      </c>
+      <c r="P10">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="Q10">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="R10">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="S10">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="T10">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="U10">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="O11">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="P11">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="Q11">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="R11">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="S11">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="T11">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="U11">
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="O12">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="P12">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="Q12">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="R12">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="S12">
+        <v>0.71</v>
+      </c>
+      <c r="T12">
+        <v>0.624</v>
+      </c>
+      <c r="U12">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16">
+        <v>0.77039999999999997</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.1333</v>
+      </c>
+      <c r="E16">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="F16">
+        <v>1.153</v>
+      </c>
+      <c r="G16">
+        <v>9.2000000000000003E-4</v>
+      </c>
+      <c r="H16">
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M16">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="O17">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="P17">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="Q17">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="R17">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="S17">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="T17">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="U17">
+        <v>0.77700000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="O18">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="P18">
+        <v>0.66</v>
+      </c>
+      <c r="Q18">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="R18">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="S18">
+        <v>0.752</v>
+      </c>
+      <c r="T18">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="U18">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="O19">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.68</v>
+      </c>
+      <c r="Q19">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="R19">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="S19">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="T19">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="U19">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23">
+        <v>0.73219999999999996</v>
+      </c>
+      <c r="D23">
+        <v>1.1707000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="F23">
+        <v>1.1902999999999999</v>
+      </c>
+      <c r="G23">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="H23">
+        <v>32</v>
+      </c>
+      <c r="I23">
+        <v>0.71679999999999999</v>
+      </c>
+      <c r="J23">
+        <v>0.80879999999999996</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24">
+        <v>0.75</v>
+      </c>
+      <c r="O24">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="P24">
+        <v>0.67</v>
+      </c>
+      <c r="Q24">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="R24">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="S24">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="T24">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="U24">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="O25">
+        <v>0.317</v>
+      </c>
+      <c r="P25">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="Q25">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="R25">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="S25">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="T25">
+        <v>0.63</v>
+      </c>
+      <c r="U25">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="O26">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="P26">
+        <v>0.62</v>
+      </c>
+      <c r="Q26">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="R26">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="S26">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="T26">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="U26">
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:21" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30">
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.1331</v>
+      </c>
+      <c r="E30">
+        <v>0.75619999999999998</v>
+      </c>
+      <c r="F30">
+        <v>1.1505000000000001</v>
+      </c>
+      <c r="G30">
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="H30">
+        <v>64</v>
+      </c>
+      <c r="I30">
+        <v>0.30759999999999998</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M30">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <v>0.79</v>
+      </c>
+      <c r="O31">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="P31">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="Q31">
+        <v>0.876</v>
+      </c>
+      <c r="R31">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="S31">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="T31">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="U31">
+        <v>0.76400000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32">
+        <v>0.72</v>
+      </c>
+      <c r="O32">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="P32">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="Q32">
+        <v>0.879</v>
+      </c>
+      <c r="R32">
+        <v>0.77</v>
+      </c>
+      <c r="S32">
+        <v>0.752</v>
+      </c>
+      <c r="T32">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="U32">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33">
+        <v>0.79</v>
+      </c>
+      <c r="O33">
+        <v>0.498</v>
+      </c>
+      <c r="P33">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="Q33">
+        <v>0.872</v>
+      </c>
+      <c r="R33">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="S33">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="T33">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="U33">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="D37">
+        <v>1.1368</v>
+      </c>
+      <c r="E37">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="F37">
+        <v>1.1580999999999999</v>
+      </c>
+      <c r="G37">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="H37">
+        <v>128</v>
+      </c>
+      <c r="I37">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="J37">
+        <v>0.32590000000000002</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M37">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N38">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="O38">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="P38">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="Q38">
+        <v>0.872</v>
+      </c>
+      <c r="R38">
+        <v>0.751</v>
+      </c>
+      <c r="S38">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="T38">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="U38">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N39">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="O39">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="P39">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="Q39">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="R39">
+        <v>0.76</v>
+      </c>
+      <c r="S39">
+        <v>0.749</v>
+      </c>
+      <c r="T39">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="U39">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="O40">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="P40">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="Q40">
+        <v>0.88</v>
+      </c>
+      <c r="R40">
+        <v>0.751</v>
+      </c>
+      <c r="S40">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="T40">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="U40">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44">
+        <v>0.7702</v>
+      </c>
+      <c r="D44">
+        <v>1.1355999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="F44">
+        <v>1.1543000000000001</v>
+      </c>
+      <c r="G44">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="H44">
+        <v>32</v>
+      </c>
+      <c r="I44">
+        <v>0.16569999999999999</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M44">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N45">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="O45">
+        <v>0.49</v>
+      </c>
+      <c r="P45">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="Q45">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="R45">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="S45">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="T45">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="U45">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N46">
+        <v>0.73</v>
+      </c>
+      <c r="O46">
+        <v>0.495</v>
+      </c>
+      <c r="P46">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="Q46">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="R46">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="S46">
+        <v>0.754</v>
+      </c>
+      <c r="T46">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="U46">
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N47">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="O47">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="P47">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="Q47">
+        <v>0.89</v>
+      </c>
+      <c r="R47">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="S47">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="T47">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="U47">
+        <v>0.76400000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:21" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51">
+        <v>0.71909999999999996</v>
+      </c>
+      <c r="D51">
+        <v>1.1861999999999999</v>
+      </c>
+      <c r="E51">
+        <v>0.7026</v>
+      </c>
+      <c r="F51">
+        <v>1.2009000000000001</v>
+      </c>
+      <c r="G51">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="H51">
+        <v>256</v>
+      </c>
+      <c r="I51">
+        <v>0.41120000000000001</v>
+      </c>
+      <c r="J51">
+        <v>0.81759999999999999</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M51">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="O52">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="P52">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="Q52">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="R52">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="S52">
+        <v>0.73</v>
+      </c>
+      <c r="T52">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="U52">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N53">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="O53">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="P53">
+        <v>0.621</v>
+      </c>
+      <c r="Q53">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="R53">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="S53">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="T53">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="U53">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N54">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="O54">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="P54">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="Q54">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="R54">
+        <v>0.69</v>
+      </c>
+      <c r="S54">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="T54">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="U54">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A37:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CDC57B-BC5E-4DF8-A65E-524FA9056D1E}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,4 +4048,412 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C2A395-5872-4D6B-9DD8-4136D9F170DD}">
+  <dimension ref="A1:T54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" customWidth="1"/>
+    <col min="19" max="20" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.74650000000000005</v>
+      </c>
+      <c r="F2">
+        <v>0.98060000000000003</v>
+      </c>
+      <c r="G2">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="H2">
+        <v>64</v>
+      </c>
+      <c r="I2">
+        <v>0.1263</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>0.999</v>
+      </c>
+      <c r="O3">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="P3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q3">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="R3">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="S3">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="T3">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>0.998</v>
+      </c>
+      <c r="O4">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="P4">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="Q4">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="R4">
+        <v>0.746</v>
+      </c>
+      <c r="S4">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="T4">
+        <v>0.746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>0.999</v>
+      </c>
+      <c r="O5">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="P5">
+        <v>0.52</v>
+      </c>
+      <c r="Q5">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="R5">
+        <v>0.747</v>
+      </c>
+      <c r="S5">
+        <v>0.621</v>
+      </c>
+      <c r="T5">
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:20" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:20" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="D16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:12" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:12" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="D30" s="2"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:12" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:12" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A37:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>